<commit_message>
Many changes at methods, introduction and impacts
</commit_message>
<xml_diff>
--- a/_bookdown_files/tables/industrie_tab3.xlsx
+++ b/_bookdown_files/tables/industrie_tab3.xlsx
@@ -27,39 +27,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Cluster Number</t>
-  </si>
-  <si>
-    <t>Cluster name</t>
-  </si>
-  <si>
-    <t>Number of Nodes (German Version)</t>
-  </si>
-  <si>
-    <t>Number of Nodes (English Version)</t>
-  </si>
-  <si>
-    <t>Internet of things &amp; manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cognition </t>
-  </si>
-  <si>
-    <t>Data, processing &amp; analytics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation  </t>
-  </si>
-  <si>
-    <t>Cloud computing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Production, product life circle &amp; flow production</t>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>1- Internet of things &amp; manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2- Cognition </t>
+  </si>
+  <si>
+    <t>3- Data, processing &amp; analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4- Automation  </t>
+  </si>
+  <si>
+    <t>5- Cloud computing</t>
+  </si>
+  <si>
+    <t>6- Production, product life circle and flow production</t>
+  </si>
+  <si>
+    <t># Nodes German</t>
+  </si>
+  <si>
+    <t># Nodes English</t>
   </si>
 </sst>
 </file>
@@ -114,16 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,108 +396,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="56" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C6" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="70" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="56" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="2">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>